<commit_message>
Configura correctamente el deploy al AWS
</commit_message>
<xml_diff>
--- a/Cuenca_conagua/uploaded_files/datos/Lluvia_media_anual.xlsx
+++ b/Cuenca_conagua/uploaded_files/datos/Lluvia_media_anual.xlsx
@@ -1,30 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PorfirioÁngel\OneDrive\Servicio_social\Docs_subir_servidor\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Lluvia media mensual, mm </t>
   </si>
@@ -111,16 +101,21 @@
   </si>
   <si>
     <t>14-15</t>
+  </si>
+  <si>
+    <t>15-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +147,137 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +290,176 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -190,11 +482,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,18 +651,67 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="39" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="52">
+    <cellStyle name="20% - Énfasis1" xfId="16" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="20" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="24" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="28" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="32" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="36" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="17" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="21" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="25" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="29" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="33" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="37" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="18" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="22" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="26" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="30" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="34" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="38" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="9" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="11" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="10" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="4" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="15" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="19" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="23" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="27" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="31" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="35" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="7" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Euro" xfId="40"/>
+    <cellStyle name="Euro 2" xfId="41"/>
+    <cellStyle name="Hipervínculo 2" xfId="42"/>
+    <cellStyle name="Incorrecto" xfId="5" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Millares 2" xfId="43"/>
+    <cellStyle name="Millares 3" xfId="44"/>
+    <cellStyle name="Millares 4" xfId="45"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="46"/>
+    <cellStyle name="Normal 2 2" xfId="47"/>
+    <cellStyle name="Normal 3" xfId="48"/>
+    <cellStyle name="Normal 4" xfId="49"/>
+    <cellStyle name="Normal 5" xfId="39"/>
+    <cellStyle name="Notas 2" xfId="50"/>
+    <cellStyle name="Porcentaje 2" xfId="51"/>
+    <cellStyle name="Salida" xfId="8" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="12" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="13" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="3" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="14" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -267,7 +760,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,7 +795,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,7 +972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,20 +983,20 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A18"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="17.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="M2" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -547,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -563,7 +1056,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -608,7 +1101,7 @@
         <v>951.80000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -653,7 +1146,7 @@
         <v>885.63</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
@@ -698,7 +1191,7 @@
         <v>553.95228863200009</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -743,7 +1236,7 @@
         <v>768.84769400000005</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -788,7 +1281,7 @@
         <v>735.7995719999999</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -833,7 +1326,7 @@
         <v>745.11709743333324</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
@@ -878,7 +1371,7 @@
         <v>660.84598600000004</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -923,7 +1416,7 @@
         <v>801.19949119400007</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -968,7 +1461,7 @@
         <v>481.71425340000002</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
@@ -1013,7 +1506,7 @@
         <v>585.90977400000008</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
@@ -1058,7 +1551,7 @@
         <v>738.93946999999991</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1596,7 @@
         <v>782.52292599999987</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
@@ -1148,85 +1641,124 @@
         <v>870.51451099999997</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8">
+        <v>4.6754859999999994</v>
+      </c>
+      <c r="C19" s="8">
+        <v>13.309269</v>
+      </c>
+      <c r="D19" s="8">
+        <v>6.7845400000000007</v>
+      </c>
+      <c r="E19" s="8">
+        <v>3.19693</v>
+      </c>
+      <c r="F19" s="8">
+        <v>21.835500000000003</v>
+      </c>
+      <c r="G19" s="8">
+        <v>10.226281999999999</v>
+      </c>
+      <c r="H19" s="8">
+        <v>42.415078999999999</v>
+      </c>
+      <c r="I19" s="8">
+        <v>117.12362299999999</v>
+      </c>
+      <c r="J19" s="8">
+        <v>170.40609000000001</v>
+      </c>
+      <c r="K19" s="8">
+        <v>202.70077000000001</v>
+      </c>
+      <c r="L19" s="8">
+        <v>80.746818000000005</v>
+      </c>
+      <c r="M19" s="8">
+        <v>31.789432000000001</v>
+      </c>
       <c r="N19" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <f>SUM(B19:M19)</f>
+        <v>705.20981900000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N20" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="N21" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="N22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="5">
-        <f>AVERAGE(B6:B18)</f>
-        <v>11.382032897435899</v>
+        <f>AVERAGE(B6:B19)</f>
+        <v>10.902993833333335</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" ref="C23:M23" si="1">AVERAGE(C6:C18)</f>
-        <v>5.5365188205128195</v>
+        <f>AVERAGE(C6:C19)</f>
+        <v>6.0917152619047608</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="1"/>
-        <v>12.808095141025644</v>
+        <f t="shared" ref="D23:M23" si="1">AVERAGE(D6:D19)</f>
+        <v>12.377841202380955</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>21.205975076923078</v>
+        <v>19.919614714285718</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="1"/>
-        <v>15.329372069230768</v>
+        <v>15.79409549285714</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="1"/>
-        <v>7.1919798256410257</v>
+        <v>7.4087156952380946</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="1"/>
-        <v>40.492138517948725</v>
+        <v>40.629491409523816</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" si="1"/>
-        <v>119.09279527179486</v>
+        <v>118.9521401095238</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="1"/>
-        <v>175.38801713846155</v>
+        <v>175.03216520000001</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>144.26948383543589</v>
+        <v>148.44314713290473</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="1"/>
-        <v>137.61776443333332</v>
+        <v>133.55555397380951</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="1"/>
-        <v>45.285293407589741</v>
+        <v>44.321303307047621</v>
       </c>
       <c r="N23" s="6">
         <f t="shared" si="0"/>
-        <v>735.5994664353334</v>
+        <v>733.42877733280955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>